<commit_message>
Time measurement results: update .xls
</commit_message>
<xml_diff>
--- a/RunTimeReport.xlsx
+++ b/RunTimeReport.xlsx
@@ -8,15 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Все правила" sheetId="1" r:id="rId1"/>
-    <sheet name="Выборочно - правила" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Pellet, Prolog, Jena, SPARQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="111">
   <si>
     <t>Запуск Stardog</t>
   </si>
@@ -206,43 +205,163 @@
     <t>Время работы правил, сек</t>
   </si>
   <si>
-    <t>s1</t>
-  </si>
-  <si>
-    <t>s2</t>
-  </si>
-  <si>
-    <t>s3</t>
-  </si>
-  <si>
-    <t>s4</t>
-  </si>
-  <si>
-    <t>s5</t>
-  </si>
-  <si>
-    <t>s6</t>
-  </si>
-  <si>
-    <t>s7</t>
-  </si>
-  <si>
-    <t>s8</t>
-  </si>
-  <si>
-    <t>s9</t>
-  </si>
-  <si>
-    <t>s10</t>
-  </si>
-  <si>
-    <t>g1</t>
-  </si>
-  <si>
-    <t>g2</t>
-  </si>
-  <si>
-    <t>Правило</t>
+    <t>Pellet 2</t>
+  </si>
+  <si>
+    <t>JAR</t>
+  </si>
+  <si>
+    <t>EXE</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>reasoner</t>
+  </si>
+  <si>
+    <t>Jena</t>
+  </si>
+  <si>
+    <t>naïve Prolog</t>
+  </si>
+  <si>
+    <t>naïve SPARQL</t>
+  </si>
+  <si>
+    <t>SWRL</t>
+  </si>
+  <si>
+    <t>Jena rules</t>
+  </si>
+  <si>
+    <t>Prolog + semweb</t>
+  </si>
+  <si>
+    <t>SPARQL select+insert</t>
+  </si>
+  <si>
+    <t>rule language</t>
+  </si>
+  <si>
+    <t>RDFS core rules location</t>
+  </si>
+  <si>
+    <t>built in</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + 4 explicit rules</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + 2 explicit rules</t>
+  </si>
+  <si>
+    <t>total rules</t>
+  </si>
+  <si>
+    <t>MIN of 5 runs, in seconds:</t>
+  </si>
+  <si>
+    <t>3.215</t>
+  </si>
+  <si>
+    <t>18.941</t>
+  </si>
+  <si>
+    <t>forward chaining</t>
+  </si>
+  <si>
+    <t>30 iterations</t>
+  </si>
+  <si>
+    <t>no chaining (iterate until nothing inferred)</t>
+  </si>
+  <si>
+    <t>error cnt</t>
+  </si>
+  <si>
+    <t>trace cnt</t>
+  </si>
+  <si>
+    <t>alg cnt</t>
+  </si>
+  <si>
+    <t>test_one</t>
+  </si>
+  <si>
+    <t>correct_branching</t>
+  </si>
+  <si>
+    <t>approx. RAM usage, Mb:</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>14 iterations</t>
+  </si>
+  <si>
+    <t>6.106</t>
+  </si>
+  <si>
+    <t>63.320</t>
+  </si>
+  <si>
+    <t>err_branching</t>
+  </si>
+  <si>
+    <t>36.599</t>
+  </si>
+  <si>
+    <t>7.516</t>
+  </si>
+  <si>
+    <t>fail (489.3)</t>
+  </si>
+  <si>
+    <t>triples init.</t>
+  </si>
+  <si>
+    <t>correct_loops</t>
+  </si>
+  <si>
+    <t>time of 1 run, in seconds:</t>
+  </si>
+  <si>
+    <t>38 iterations</t>
+  </si>
+  <si>
+    <t>467.581</t>
+  </si>
+  <si>
+    <t>triples result</t>
+  </si>
+  <si>
+    <t>118.696</t>
+  </si>
+  <si>
+    <t>15.435</t>
+  </si>
+  <si>
+    <t>18 iterations</t>
+  </si>
+  <si>
+    <t>fail (2111)</t>
+  </si>
+  <si>
+    <t>5.956</t>
+  </si>
+  <si>
+    <t>6.508</t>
+  </si>
+  <si>
+    <t>4.608</t>
+  </si>
+  <si>
+    <t>2.112</t>
+  </si>
+  <si>
+    <t>36.382</t>
   </si>
 </sst>
 </file>
@@ -300,7 +419,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,8 +462,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -352,11 +477,82 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -383,6 +579,28 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1371,71 +1589,414 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M2"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:M1048576"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="13" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="28" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="29" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="28" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" style="29" customWidth="1"/>
+    <col min="11" max="16" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G1" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="25"/>
+      <c r="I1" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="27"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="G5" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="K2" t="s">
+      <c r="H5" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="L2" t="s">
+      <c r="I5" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="M2" t="s">
+      <c r="J5" s="29" t="s">
         <v>69</v>
       </c>
     </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="28">
+        <v>98</v>
+      </c>
+      <c r="H7" s="29">
+        <v>102</v>
+      </c>
+      <c r="I7" s="28">
+        <v>98</v>
+      </c>
+      <c r="J7" s="29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="40"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="33">
+        <v>1</v>
+      </c>
+      <c r="C11" s="33">
+        <v>1</v>
+      </c>
+      <c r="D11" s="33">
+        <v>5</v>
+      </c>
+      <c r="E11" s="33">
+        <v>725</v>
+      </c>
+      <c r="F11" s="33">
+        <v>1379</v>
+      </c>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="J12" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="28">
+        <v>840</v>
+      </c>
+      <c r="H13" s="29">
+        <v>70</v>
+      </c>
+      <c r="I13" s="28">
+        <v>7.5</v>
+      </c>
+      <c r="J13" s="29">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="33">
+        <v>4</v>
+      </c>
+      <c r="C16" s="33">
+        <v>23</v>
+      </c>
+      <c r="D16" s="33">
+        <v>0</v>
+      </c>
+      <c r="E16" s="33">
+        <v>3095</v>
+      </c>
+      <c r="F16" s="33">
+        <v>5981</v>
+      </c>
+      <c r="G16" s="34"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="J16" s="35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" s="28">
+        <v>1553</v>
+      </c>
+      <c r="H18" s="29">
+        <v>215</v>
+      </c>
+      <c r="I18" s="28">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J18" s="29">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="33">
+        <v>3</v>
+      </c>
+      <c r="C21" s="33">
+        <v>54</v>
+      </c>
+      <c r="D21" s="33">
+        <v>98</v>
+      </c>
+      <c r="E21" s="33">
+        <v>7571</v>
+      </c>
+      <c r="F21" s="33">
+        <v>19462</v>
+      </c>
+      <c r="G21" s="34"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="J21" s="35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="J22" s="29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="H23" s="29">
+        <v>467</v>
+      </c>
+      <c r="I23" s="28">
+        <v>9.9</v>
+      </c>
+      <c r="J23" s="29">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="33">
+        <v>5</v>
+      </c>
+      <c r="C26" s="33">
+        <v>86</v>
+      </c>
+      <c r="D26" s="33">
+        <v>0</v>
+      </c>
+      <c r="E26" s="33">
+        <v>22236</v>
+      </c>
+      <c r="F26" s="38">
+        <v>58350</v>
+      </c>
+      <c r="G26" s="34"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="J26" s="35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="J27" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H28" s="29">
+        <v>1776</v>
+      </c>
+      <c r="I28" s="28">
+        <v>15</v>
+      </c>
+      <c r="J28" s="29">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E31" s="37"/>
+      <c r="G31" s="36"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>